<commit_message>
trying to impliment a smoothing on line
Signed-off-by: akudlacek <7029639+akudlacek@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/table blender.xlsx
+++ b/table blender.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akudlacek\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akudlacek\Downloads\cummins_tuning_calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11480642-2AB0-465A-85E6-74589DF34513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF57BF83-B7D8-460A-871C-1BC17AA75E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D6206C45-3FE7-4868-8A95-239C7ED022B7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t>Table 1</t>
   </si>
@@ -70,13 +70,19 @@
   <si>
     <t>y</t>
   </si>
+  <si>
+    <t>Distance from line</t>
+  </si>
+  <si>
+    <t>Blended</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -109,12 +115,62 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -515,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7647053-835B-421E-A05A-5E37237959C0}">
-  <dimension ref="A1:U69"/>
+  <dimension ref="A1:U115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S45" sqref="S45"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97:Q115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4231,8 +4287,1911 @@
         <v>-1411.7647058823532</v>
       </c>
     </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>3</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <v>10</v>
+      </c>
+      <c r="D73">
+        <v>20</v>
+      </c>
+      <c r="E73">
+        <v>30</v>
+      </c>
+      <c r="F73">
+        <v>45</v>
+      </c>
+      <c r="G73">
+        <v>53.1</v>
+      </c>
+      <c r="H73">
+        <v>59.2</v>
+      </c>
+      <c r="I73">
+        <v>65.3</v>
+      </c>
+      <c r="J73">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="K73">
+        <v>77.5</v>
+      </c>
+      <c r="L73">
+        <v>86.7</v>
+      </c>
+      <c r="M73">
+        <v>92.7</v>
+      </c>
+      <c r="N73">
+        <v>95.9</v>
+      </c>
+      <c r="O73">
+        <v>98.9</v>
+      </c>
+      <c r="P73">
+        <v>105</v>
+      </c>
+      <c r="Q73">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>620</v>
+      </c>
+      <c r="B74" s="1">
+        <f>ABS($U$53*B$73-$A74-$U$53*$T$50+$U$50)/SQRT($U$53^2+1)</f>
+        <v>116.79863203522085</v>
+      </c>
+      <c r="C74" s="1">
+        <f t="shared" ref="C74:Q89" si="21">ABS($U$53*C$73-$A74-$U$53*$T$50+$U$50)/SQRT($U$53^2+1)</f>
+        <v>106.80088908335091</v>
+      </c>
+      <c r="D74" s="1">
+        <f t="shared" si="21"/>
+        <v>96.803146131480929</v>
+      </c>
+      <c r="E74" s="1">
+        <f t="shared" si="21"/>
+        <v>86.805403179610963</v>
+      </c>
+      <c r="F74" s="1">
+        <f t="shared" si="21"/>
+        <v>71.808788751806006</v>
+      </c>
+      <c r="G74" s="1">
+        <f t="shared" si="21"/>
+        <v>63.710616960791349</v>
+      </c>
+      <c r="H74" s="1">
+        <f t="shared" si="21"/>
+        <v>57.611993760150668</v>
+      </c>
+      <c r="I74" s="1">
+        <f t="shared" si="21"/>
+        <v>51.513370559509994</v>
+      </c>
+      <c r="J74" s="1">
+        <f t="shared" si="21"/>
+        <v>45.414747358869306</v>
+      </c>
+      <c r="K74" s="1">
+        <f t="shared" si="21"/>
+        <v>39.316124158228618</v>
+      </c>
+      <c r="L74" s="1">
+        <f t="shared" si="21"/>
+        <v>30.11820064250827</v>
+      </c>
+      <c r="M74" s="1">
+        <f t="shared" si="21"/>
+        <v>24.119554871386281</v>
+      </c>
+      <c r="N74" s="1">
+        <f t="shared" si="21"/>
+        <v>20.920277126787884</v>
+      </c>
+      <c r="O74" s="1">
+        <f t="shared" si="21"/>
+        <v>17.920954241226898</v>
+      </c>
+      <c r="P74" s="1">
+        <f t="shared" si="21"/>
+        <v>11.822331040586223</v>
+      </c>
+      <c r="Q74" s="1">
+        <f t="shared" si="21"/>
+        <v>43.165255194698574</v>
+      </c>
+      <c r="R74" s="1"/>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>650</v>
+      </c>
+      <c r="B75" s="1">
+        <f t="shared" ref="B75:Q92" si="22">ABS($U$53*B$73-$A75-$U$53*$T$50+$U$50)/SQRT($U$53^2+1)</f>
+        <v>116.16127592203914</v>
+      </c>
+      <c r="C75" s="1">
+        <f t="shared" si="21"/>
+        <v>106.16353297016919</v>
+      </c>
+      <c r="D75" s="1">
+        <f t="shared" si="21"/>
+        <v>96.165790018299219</v>
+      </c>
+      <c r="E75" s="1">
+        <f t="shared" si="21"/>
+        <v>86.168047066429253</v>
+      </c>
+      <c r="F75" s="1">
+        <f t="shared" si="21"/>
+        <v>71.171432638624296</v>
+      </c>
+      <c r="G75" s="1">
+        <f t="shared" si="21"/>
+        <v>63.073260847609639</v>
+      </c>
+      <c r="H75" s="1">
+        <f t="shared" si="21"/>
+        <v>56.974637646968958</v>
+      </c>
+      <c r="I75" s="1">
+        <f t="shared" si="21"/>
+        <v>50.876014446328284</v>
+      </c>
+      <c r="J75" s="1">
+        <f t="shared" si="21"/>
+        <v>44.777391245687596</v>
+      </c>
+      <c r="K75" s="1">
+        <f t="shared" si="21"/>
+        <v>38.678768045046908</v>
+      </c>
+      <c r="L75" s="1">
+        <f t="shared" si="21"/>
+        <v>29.480844529326561</v>
+      </c>
+      <c r="M75" s="1">
+        <f t="shared" si="21"/>
+        <v>23.482198758204571</v>
+      </c>
+      <c r="N75" s="1">
+        <f t="shared" si="21"/>
+        <v>20.282921013606174</v>
+      </c>
+      <c r="O75" s="1">
+        <f t="shared" si="21"/>
+        <v>17.283598128045188</v>
+      </c>
+      <c r="P75" s="1">
+        <f t="shared" si="21"/>
+        <v>11.184974927404513</v>
+      </c>
+      <c r="Q75" s="1">
+        <f t="shared" si="21"/>
+        <v>43.802611307880284</v>
+      </c>
+      <c r="R75" s="1"/>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>800</v>
+      </c>
+      <c r="B76" s="1">
+        <f t="shared" si="22"/>
+        <v>112.97449535613059</v>
+      </c>
+      <c r="C76" s="1">
+        <f t="shared" si="21"/>
+        <v>102.97675240426064</v>
+      </c>
+      <c r="D76" s="1">
+        <f t="shared" si="21"/>
+        <v>92.97900945239067</v>
+      </c>
+      <c r="E76" s="1">
+        <f t="shared" si="21"/>
+        <v>82.981266500520704</v>
+      </c>
+      <c r="F76" s="1">
+        <f t="shared" si="21"/>
+        <v>67.984652072715747</v>
+      </c>
+      <c r="G76" s="1">
+        <f t="shared" si="21"/>
+        <v>59.886480281701083</v>
+      </c>
+      <c r="H76" s="1">
+        <f t="shared" si="21"/>
+        <v>53.787857081060409</v>
+      </c>
+      <c r="I76" s="1">
+        <f t="shared" si="21"/>
+        <v>47.689233880419728</v>
+      </c>
+      <c r="J76" s="1">
+        <f t="shared" si="21"/>
+        <v>41.590610679779054</v>
+      </c>
+      <c r="K76" s="1">
+        <f t="shared" si="21"/>
+        <v>35.491987479138359</v>
+      </c>
+      <c r="L76" s="1">
+        <f t="shared" si="21"/>
+        <v>26.294063963418012</v>
+      </c>
+      <c r="M76" s="1">
+        <f t="shared" si="21"/>
+        <v>20.295418192296019</v>
+      </c>
+      <c r="N76" s="1">
+        <f t="shared" si="21"/>
+        <v>17.096140447697625</v>
+      </c>
+      <c r="O76" s="1">
+        <f t="shared" si="21"/>
+        <v>14.096817562136637</v>
+      </c>
+      <c r="P76" s="1">
+        <f t="shared" si="21"/>
+        <v>7.9981943614959619</v>
+      </c>
+      <c r="Q76" s="1">
+        <f t="shared" si="21"/>
+        <v>46.989391873788833</v>
+      </c>
+      <c r="R76" s="1"/>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>1000</v>
+      </c>
+      <c r="B77" s="1">
+        <f t="shared" si="22"/>
+        <v>108.72545460158587</v>
+      </c>
+      <c r="C77" s="1">
+        <f t="shared" si="21"/>
+        <v>98.727711649715914</v>
+      </c>
+      <c r="D77" s="1">
+        <f t="shared" si="21"/>
+        <v>88.729968697845933</v>
+      </c>
+      <c r="E77" s="1">
+        <f t="shared" si="21"/>
+        <v>78.732225745975967</v>
+      </c>
+      <c r="F77" s="1">
+        <f t="shared" si="21"/>
+        <v>63.735611318171017</v>
+      </c>
+      <c r="G77" s="1">
+        <f t="shared" si="21"/>
+        <v>55.637439527156353</v>
+      </c>
+      <c r="H77" s="1">
+        <f t="shared" si="21"/>
+        <v>49.538816326515672</v>
+      </c>
+      <c r="I77" s="1">
+        <f t="shared" si="21"/>
+        <v>43.440193125874998</v>
+      </c>
+      <c r="J77" s="1">
+        <f t="shared" si="21"/>
+        <v>37.341569925234317</v>
+      </c>
+      <c r="K77" s="1">
+        <f t="shared" si="21"/>
+        <v>31.242946724593626</v>
+      </c>
+      <c r="L77" s="1">
+        <f t="shared" si="21"/>
+        <v>22.045023208873275</v>
+      </c>
+      <c r="M77" s="1">
+        <f t="shared" si="21"/>
+        <v>16.046377437751286</v>
+      </c>
+      <c r="N77" s="1">
+        <f t="shared" si="21"/>
+        <v>12.84709969315289</v>
+      </c>
+      <c r="O77" s="1">
+        <f t="shared" si="21"/>
+        <v>9.8477768075919041</v>
+      </c>
+      <c r="P77" s="1">
+        <f t="shared" si="21"/>
+        <v>3.7491536069512272</v>
+      </c>
+      <c r="Q77" s="1">
+        <f t="shared" si="21"/>
+        <v>51.23843262833357</v>
+      </c>
+      <c r="R77" s="1"/>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>1200</v>
+      </c>
+      <c r="B78" s="1">
+        <f t="shared" si="22"/>
+        <v>104.47641384704113</v>
+      </c>
+      <c r="C78" s="1">
+        <f t="shared" si="21"/>
+        <v>94.478670895171177</v>
+      </c>
+      <c r="D78" s="1">
+        <f t="shared" si="21"/>
+        <v>84.480927943301197</v>
+      </c>
+      <c r="E78" s="1">
+        <f t="shared" si="21"/>
+        <v>74.48318499143123</v>
+      </c>
+      <c r="F78" s="1">
+        <f t="shared" si="21"/>
+        <v>59.48657056362628</v>
+      </c>
+      <c r="G78" s="1">
+        <f t="shared" si="21"/>
+        <v>51.388398772611616</v>
+      </c>
+      <c r="H78" s="1">
+        <f t="shared" si="21"/>
+        <v>45.289775571970942</v>
+      </c>
+      <c r="I78" s="1">
+        <f t="shared" si="21"/>
+        <v>39.191152371330261</v>
+      </c>
+      <c r="J78" s="1">
+        <f t="shared" si="21"/>
+        <v>33.092529170689588</v>
+      </c>
+      <c r="K78" s="1">
+        <f t="shared" si="21"/>
+        <v>26.993905970048889</v>
+      </c>
+      <c r="L78" s="1">
+        <f t="shared" si="21"/>
+        <v>17.795982454328541</v>
+      </c>
+      <c r="M78" s="1">
+        <f t="shared" si="21"/>
+        <v>11.79733668320655</v>
+      </c>
+      <c r="N78" s="1">
+        <f t="shared" si="21"/>
+        <v>8.5980589386081547</v>
+      </c>
+      <c r="O78" s="1">
+        <f t="shared" si="21"/>
+        <v>5.598736053047169</v>
+      </c>
+      <c r="P78" s="1">
+        <f t="shared" si="21"/>
+        <v>0.49988714759350728</v>
+      </c>
+      <c r="Q78" s="1">
+        <f t="shared" si="21"/>
+        <v>55.487473382878299</v>
+      </c>
+      <c r="R78" s="1"/>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>1400</v>
+      </c>
+      <c r="B79" s="1">
+        <f t="shared" si="22"/>
+        <v>100.22737309249639</v>
+      </c>
+      <c r="C79" s="1">
+        <f t="shared" si="21"/>
+        <v>90.22963014062644</v>
+      </c>
+      <c r="D79" s="1">
+        <f t="shared" si="21"/>
+        <v>80.231887188756474</v>
+      </c>
+      <c r="E79" s="1">
+        <f t="shared" si="21"/>
+        <v>70.234144236886493</v>
+      </c>
+      <c r="F79" s="1">
+        <f t="shared" si="21"/>
+        <v>55.237529809081551</v>
+      </c>
+      <c r="G79" s="1">
+        <f t="shared" si="21"/>
+        <v>47.139358018066879</v>
+      </c>
+      <c r="H79" s="1">
+        <f t="shared" si="21"/>
+        <v>41.040734817426205</v>
+      </c>
+      <c r="I79" s="1">
+        <f t="shared" si="21"/>
+        <v>34.942111616785525</v>
+      </c>
+      <c r="J79" s="1">
+        <f t="shared" si="21"/>
+        <v>28.843488416144851</v>
+      </c>
+      <c r="K79" s="1">
+        <f t="shared" si="21"/>
+        <v>22.744865215504156</v>
+      </c>
+      <c r="L79" s="1">
+        <f t="shared" si="21"/>
+        <v>13.546941699783808</v>
+      </c>
+      <c r="M79" s="1">
+        <f t="shared" si="21"/>
+        <v>7.5482959286618163</v>
+      </c>
+      <c r="N79" s="1">
+        <f t="shared" si="21"/>
+        <v>4.3490181840634206</v>
+      </c>
+      <c r="O79" s="1">
+        <f t="shared" si="21"/>
+        <v>1.3496952985024349</v>
+      </c>
+      <c r="P79" s="1">
+        <f t="shared" si="21"/>
+        <v>4.7489279021382416</v>
+      </c>
+      <c r="Q79" s="1">
+        <f t="shared" si="21"/>
+        <v>59.736514137423036</v>
+      </c>
+      <c r="R79" s="1"/>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>1550</v>
+      </c>
+      <c r="B80" s="1">
+        <f t="shared" si="22"/>
+        <v>97.040592526587844</v>
+      </c>
+      <c r="C80" s="1">
+        <f t="shared" si="21"/>
+        <v>87.042849574717891</v>
+      </c>
+      <c r="D80" s="1">
+        <f t="shared" si="21"/>
+        <v>77.045106622847911</v>
+      </c>
+      <c r="E80" s="1">
+        <f t="shared" si="21"/>
+        <v>67.047363670977944</v>
+      </c>
+      <c r="F80" s="1">
+        <f t="shared" si="21"/>
+        <v>52.050749243172994</v>
+      </c>
+      <c r="G80" s="1">
+        <f t="shared" si="21"/>
+        <v>43.95257745215833</v>
+      </c>
+      <c r="H80" s="1">
+        <f t="shared" si="21"/>
+        <v>37.853954251517656</v>
+      </c>
+      <c r="I80" s="1">
+        <f t="shared" si="21"/>
+        <v>31.755331050876975</v>
+      </c>
+      <c r="J80" s="1">
+        <f t="shared" si="21"/>
+        <v>25.656707850236302</v>
+      </c>
+      <c r="K80" s="1">
+        <f t="shared" si="21"/>
+        <v>19.558084649595603</v>
+      </c>
+      <c r="L80" s="1">
+        <f t="shared" si="21"/>
+        <v>10.360161133875257</v>
+      </c>
+      <c r="M80" s="1">
+        <f t="shared" si="21"/>
+        <v>4.3615153627532655</v>
+      </c>
+      <c r="N80" s="1">
+        <f t="shared" si="21"/>
+        <v>1.1622376181548697</v>
+      </c>
+      <c r="O80" s="1">
+        <f t="shared" si="21"/>
+        <v>1.837085267406116</v>
+      </c>
+      <c r="P80" s="1">
+        <f t="shared" si="21"/>
+        <v>7.9357084680467924</v>
+      </c>
+      <c r="Q80" s="1">
+        <f t="shared" si="21"/>
+        <v>62.923294703331585</v>
+      </c>
+      <c r="R80" s="1"/>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>1700</v>
+      </c>
+      <c r="B81" s="1">
+        <f t="shared" si="22"/>
+        <v>93.853811960679295</v>
+      </c>
+      <c r="C81" s="1">
+        <f t="shared" si="21"/>
+        <v>83.856069008809328</v>
+      </c>
+      <c r="D81" s="1">
+        <f t="shared" si="21"/>
+        <v>73.858326056939362</v>
+      </c>
+      <c r="E81" s="1">
+        <f t="shared" si="21"/>
+        <v>63.860583105069395</v>
+      </c>
+      <c r="F81" s="1">
+        <f t="shared" si="21"/>
+        <v>48.863968677264445</v>
+      </c>
+      <c r="G81" s="1">
+        <f t="shared" si="21"/>
+        <v>40.765796886249781</v>
+      </c>
+      <c r="H81" s="1">
+        <f t="shared" si="21"/>
+        <v>34.6671736856091</v>
+      </c>
+      <c r="I81" s="1">
+        <f t="shared" si="21"/>
+        <v>28.568550484968426</v>
+      </c>
+      <c r="J81" s="1">
+        <f t="shared" si="21"/>
+        <v>22.469927284327749</v>
+      </c>
+      <c r="K81" s="1">
+        <f t="shared" si="21"/>
+        <v>16.371304083687054</v>
+      </c>
+      <c r="L81" s="1">
+        <f t="shared" si="21"/>
+        <v>7.1733805679667055</v>
+      </c>
+      <c r="M81" s="1">
+        <f t="shared" si="21"/>
+        <v>1.174734796844715</v>
+      </c>
+      <c r="N81" s="1">
+        <f t="shared" si="21"/>
+        <v>2.0245429477536812</v>
+      </c>
+      <c r="O81" s="1">
+        <f t="shared" si="21"/>
+        <v>5.0238658333146669</v>
+      </c>
+      <c r="P81" s="1">
+        <f t="shared" si="21"/>
+        <v>11.122489033955343</v>
+      </c>
+      <c r="Q81" s="1">
+        <f t="shared" si="21"/>
+        <v>66.110075269240141</v>
+      </c>
+      <c r="R81" s="1"/>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>1800</v>
+      </c>
+      <c r="B82" s="1">
+        <f t="shared" si="22"/>
+        <v>91.729291583406919</v>
+      </c>
+      <c r="C82" s="1">
+        <f t="shared" si="21"/>
+        <v>81.731548631536967</v>
+      </c>
+      <c r="D82" s="1">
+        <f t="shared" si="21"/>
+        <v>71.733805679667</v>
+      </c>
+      <c r="E82" s="1">
+        <f t="shared" si="21"/>
+        <v>61.736062727797027</v>
+      </c>
+      <c r="F82" s="1">
+        <f t="shared" si="21"/>
+        <v>46.739448299992077</v>
+      </c>
+      <c r="G82" s="1">
+        <f t="shared" si="21"/>
+        <v>38.641276508977413</v>
+      </c>
+      <c r="H82" s="1">
+        <f t="shared" si="21"/>
+        <v>32.542653308336739</v>
+      </c>
+      <c r="I82" s="1">
+        <f t="shared" si="21"/>
+        <v>26.444030107696058</v>
+      </c>
+      <c r="J82" s="1">
+        <f t="shared" si="21"/>
+        <v>20.345406907055384</v>
+      </c>
+      <c r="K82" s="1">
+        <f t="shared" si="21"/>
+        <v>14.246783706414687</v>
+      </c>
+      <c r="L82" s="1">
+        <f t="shared" si="21"/>
+        <v>5.048860190694338</v>
+      </c>
+      <c r="M82" s="1">
+        <f t="shared" si="21"/>
+        <v>0.94978558042765227</v>
+      </c>
+      <c r="N82" s="1">
+        <f t="shared" si="21"/>
+        <v>4.1490633250260487</v>
+      </c>
+      <c r="O82" s="1">
+        <f t="shared" si="21"/>
+        <v>7.1483862105870344</v>
+      </c>
+      <c r="P82" s="1">
+        <f t="shared" si="21"/>
+        <v>13.24700941122771</v>
+      </c>
+      <c r="Q82" s="1">
+        <f t="shared" si="21"/>
+        <v>68.234595646512503</v>
+      </c>
+      <c r="R82" s="1"/>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>2000</v>
+      </c>
+      <c r="B83" s="1">
+        <f t="shared" si="22"/>
+        <v>87.480250828862182</v>
+      </c>
+      <c r="C83" s="1">
+        <f t="shared" si="21"/>
+        <v>77.48250787699223</v>
+      </c>
+      <c r="D83" s="1">
+        <f t="shared" si="21"/>
+        <v>67.484764925122263</v>
+      </c>
+      <c r="E83" s="1">
+        <f t="shared" si="21"/>
+        <v>57.48702197325229</v>
+      </c>
+      <c r="F83" s="1">
+        <f t="shared" si="21"/>
+        <v>42.490407545447347</v>
+      </c>
+      <c r="G83" s="1">
+        <f t="shared" si="21"/>
+        <v>34.392235754432676</v>
+      </c>
+      <c r="H83" s="1">
+        <f t="shared" si="21"/>
+        <v>28.293612553792002</v>
+      </c>
+      <c r="I83" s="1">
+        <f t="shared" si="21"/>
+        <v>22.194989353151325</v>
+      </c>
+      <c r="J83" s="1">
+        <f t="shared" si="21"/>
+        <v>16.096366152510647</v>
+      </c>
+      <c r="K83" s="1">
+        <f t="shared" si="21"/>
+        <v>9.9977429518699523</v>
+      </c>
+      <c r="L83" s="1">
+        <f t="shared" si="21"/>
+        <v>0.79981943614960394</v>
+      </c>
+      <c r="M83" s="1">
+        <f t="shared" si="21"/>
+        <v>5.1988263349723871</v>
+      </c>
+      <c r="N83" s="1">
+        <f t="shared" si="21"/>
+        <v>8.3981040795707838</v>
+      </c>
+      <c r="O83" s="1">
+        <f t="shared" si="21"/>
+        <v>11.397426965131769</v>
+      </c>
+      <c r="P83" s="1">
+        <f t="shared" si="21"/>
+        <v>17.496050165772445</v>
+      </c>
+      <c r="Q83" s="1">
+        <f t="shared" si="21"/>
+        <v>72.48363640105724</v>
+      </c>
+      <c r="R83" s="1"/>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>2200</v>
+      </c>
+      <c r="B84" s="1">
+        <f t="shared" si="22"/>
+        <v>83.23121007431746</v>
+      </c>
+      <c r="C84" s="1">
+        <f t="shared" si="21"/>
+        <v>73.233467122447493</v>
+      </c>
+      <c r="D84" s="1">
+        <f t="shared" si="21"/>
+        <v>63.235724170577527</v>
+      </c>
+      <c r="E84" s="1">
+        <f t="shared" si="21"/>
+        <v>53.23798121870756</v>
+      </c>
+      <c r="F84" s="1">
+        <f t="shared" si="21"/>
+        <v>38.24136679090261</v>
+      </c>
+      <c r="G84" s="1">
+        <f t="shared" si="21"/>
+        <v>30.143194999887942</v>
+      </c>
+      <c r="H84" s="1">
+        <f t="shared" si="21"/>
+        <v>24.044571799247265</v>
+      </c>
+      <c r="I84" s="1">
+        <f t="shared" si="21"/>
+        <v>17.945948598606591</v>
+      </c>
+      <c r="J84" s="1">
+        <f t="shared" si="21"/>
+        <v>11.847325397965914</v>
+      </c>
+      <c r="K84" s="1">
+        <f t="shared" si="21"/>
+        <v>5.7487021973252173</v>
+      </c>
+      <c r="L84" s="1">
+        <f t="shared" si="21"/>
+        <v>3.4492213183951308</v>
+      </c>
+      <c r="M84" s="1">
+        <f t="shared" si="21"/>
+        <v>9.4478670895171213</v>
+      </c>
+      <c r="N84" s="1">
+        <f t="shared" si="21"/>
+        <v>12.647144834115517</v>
+      </c>
+      <c r="O84" s="1">
+        <f t="shared" si="21"/>
+        <v>15.646467719676503</v>
+      </c>
+      <c r="P84" s="1">
+        <f t="shared" si="21"/>
+        <v>21.745090920317178</v>
+      </c>
+      <c r="Q84" s="1">
+        <f t="shared" si="21"/>
+        <v>76.732677155601976</v>
+      </c>
+      <c r="R84" s="1"/>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>2400</v>
+      </c>
+      <c r="B85" s="1">
+        <f t="shared" si="22"/>
+        <v>78.982169319772723</v>
+      </c>
+      <c r="C85" s="1">
+        <f t="shared" si="21"/>
+        <v>68.984426367902756</v>
+      </c>
+      <c r="D85" s="1">
+        <f t="shared" si="21"/>
+        <v>58.986683416032797</v>
+      </c>
+      <c r="E85" s="1">
+        <f t="shared" si="21"/>
+        <v>48.988940464162823</v>
+      </c>
+      <c r="F85" s="1">
+        <f t="shared" si="21"/>
+        <v>33.992326036357873</v>
+      </c>
+      <c r="G85" s="1">
+        <f t="shared" si="21"/>
+        <v>25.894154245343209</v>
+      </c>
+      <c r="H85" s="1">
+        <f t="shared" si="21"/>
+        <v>19.795531044702532</v>
+      </c>
+      <c r="I85" s="1">
+        <f t="shared" si="21"/>
+        <v>13.696907844061856</v>
+      </c>
+      <c r="J85" s="1">
+        <f t="shared" si="21"/>
+        <v>7.598284643421179</v>
+      </c>
+      <c r="K85" s="1">
+        <f t="shared" si="21"/>
+        <v>1.4996614427804831</v>
+      </c>
+      <c r="L85" s="1">
+        <f t="shared" si="21"/>
+        <v>7.6982620729398654</v>
+      </c>
+      <c r="M85" s="1">
+        <f t="shared" si="21"/>
+        <v>13.696907844061856</v>
+      </c>
+      <c r="N85" s="1">
+        <f t="shared" si="21"/>
+        <v>16.896185588660252</v>
+      </c>
+      <c r="O85" s="1">
+        <f t="shared" si="21"/>
+        <v>19.895508474221238</v>
+      </c>
+      <c r="P85" s="1">
+        <f t="shared" si="21"/>
+        <v>25.994131674861915</v>
+      </c>
+      <c r="Q85" s="1">
+        <f t="shared" si="21"/>
+        <v>80.981717910146713</v>
+      </c>
+      <c r="R85" s="1"/>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>2600</v>
+      </c>
+      <c r="B86" s="1">
+        <f t="shared" si="22"/>
+        <v>74.733128565227986</v>
+      </c>
+      <c r="C86" s="1">
+        <f t="shared" si="21"/>
+        <v>64.735385613358019</v>
+      </c>
+      <c r="D86" s="1">
+        <f t="shared" si="21"/>
+        <v>54.73764266148806</v>
+      </c>
+      <c r="E86" s="1">
+        <f t="shared" si="21"/>
+        <v>44.739899709618086</v>
+      </c>
+      <c r="F86" s="1">
+        <f t="shared" si="21"/>
+        <v>29.74328528181314</v>
+      </c>
+      <c r="G86" s="1">
+        <f t="shared" si="21"/>
+        <v>21.645113490798476</v>
+      </c>
+      <c r="H86" s="1">
+        <f t="shared" si="21"/>
+        <v>15.546490290157799</v>
+      </c>
+      <c r="I86" s="1">
+        <f t="shared" si="21"/>
+        <v>9.4478670895171213</v>
+      </c>
+      <c r="J86" s="1">
+        <f t="shared" si="21"/>
+        <v>3.3492438888764444</v>
+      </c>
+      <c r="K86" s="1">
+        <f t="shared" si="21"/>
+        <v>2.7493793117642511</v>
+      </c>
+      <c r="L86" s="1">
+        <f t="shared" si="21"/>
+        <v>11.947302827484599</v>
+      </c>
+      <c r="M86" s="1">
+        <f t="shared" si="21"/>
+        <v>17.945948598606591</v>
+      </c>
+      <c r="N86" s="1">
+        <f t="shared" si="21"/>
+        <v>21.145226343204985</v>
+      </c>
+      <c r="O86" s="1">
+        <f t="shared" si="21"/>
+        <v>24.144549228765971</v>
+      </c>
+      <c r="P86" s="1">
+        <f t="shared" si="21"/>
+        <v>30.243172429406648</v>
+      </c>
+      <c r="Q86" s="1">
+        <f t="shared" si="21"/>
+        <v>85.23075866469145</v>
+      </c>
+      <c r="R86" s="1"/>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>2800</v>
+      </c>
+      <c r="B87" s="1">
+        <f t="shared" si="22"/>
+        <v>70.484087810683249</v>
+      </c>
+      <c r="C87" s="1">
+        <f t="shared" si="21"/>
+        <v>60.48634485881329</v>
+      </c>
+      <c r="D87" s="1">
+        <f t="shared" si="21"/>
+        <v>50.488601906943323</v>
+      </c>
+      <c r="E87" s="1">
+        <f t="shared" si="21"/>
+        <v>40.490858955073357</v>
+      </c>
+      <c r="F87" s="1">
+        <f t="shared" si="21"/>
+        <v>25.494244527268407</v>
+      </c>
+      <c r="G87" s="1">
+        <f t="shared" si="21"/>
+        <v>17.396072736253739</v>
+      </c>
+      <c r="H87" s="1">
+        <f t="shared" si="21"/>
+        <v>11.297449535613064</v>
+      </c>
+      <c r="I87" s="1">
+        <f t="shared" si="21"/>
+        <v>5.1988263349723871</v>
+      </c>
+      <c r="J87" s="1">
+        <f t="shared" si="21"/>
+        <v>0.89979686566828987</v>
+      </c>
+      <c r="K87" s="1">
+        <f t="shared" si="21"/>
+        <v>6.9984200663089862</v>
+      </c>
+      <c r="L87" s="1">
+        <f t="shared" si="21"/>
+        <v>16.196343582029336</v>
+      </c>
+      <c r="M87" s="1">
+        <f t="shared" si="21"/>
+        <v>22.194989353151325</v>
+      </c>
+      <c r="N87" s="1">
+        <f t="shared" si="21"/>
+        <v>25.394267097749722</v>
+      </c>
+      <c r="O87" s="1">
+        <f t="shared" si="21"/>
+        <v>28.393589983310708</v>
+      </c>
+      <c r="P87" s="1">
+        <f t="shared" si="21"/>
+        <v>34.492213183951385</v>
+      </c>
+      <c r="Q87" s="1">
+        <f t="shared" si="21"/>
+        <v>89.479799419236173</v>
+      </c>
+      <c r="R87" s="1"/>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>2900</v>
+      </c>
+      <c r="B88" s="1">
+        <f t="shared" si="22"/>
+        <v>68.359567433410888</v>
+      </c>
+      <c r="C88" s="1">
+        <f t="shared" si="21"/>
+        <v>58.361824481540921</v>
+      </c>
+      <c r="D88" s="1">
+        <f t="shared" si="21"/>
+        <v>48.364081529670962</v>
+      </c>
+      <c r="E88" s="1">
+        <f t="shared" si="21"/>
+        <v>38.366338577800988</v>
+      </c>
+      <c r="F88" s="1">
+        <f t="shared" si="21"/>
+        <v>23.369724149996038</v>
+      </c>
+      <c r="G88" s="1">
+        <f t="shared" si="21"/>
+        <v>15.271552358981372</v>
+      </c>
+      <c r="H88" s="1">
+        <f t="shared" si="21"/>
+        <v>9.1729291583406969</v>
+      </c>
+      <c r="I88" s="1">
+        <f t="shared" si="21"/>
+        <v>3.0743059577000196</v>
+      </c>
+      <c r="J88" s="1">
+        <f t="shared" si="21"/>
+        <v>3.0243172429406573</v>
+      </c>
+      <c r="K88" s="1">
+        <f t="shared" si="21"/>
+        <v>9.1229404435813528</v>
+      </c>
+      <c r="L88" s="1">
+        <f t="shared" si="21"/>
+        <v>18.3208639593017</v>
+      </c>
+      <c r="M88" s="1">
+        <f t="shared" si="21"/>
+        <v>24.319509730423693</v>
+      </c>
+      <c r="N88" s="1">
+        <f t="shared" si="21"/>
+        <v>27.518787475022087</v>
+      </c>
+      <c r="O88" s="1">
+        <f t="shared" si="21"/>
+        <v>30.518110360583073</v>
+      </c>
+      <c r="P88" s="1">
+        <f t="shared" si="21"/>
+        <v>36.616733561223754</v>
+      </c>
+      <c r="Q88" s="1">
+        <f t="shared" si="21"/>
+        <v>91.604319796508548</v>
+      </c>
+      <c r="R88" s="1"/>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>3000</v>
+      </c>
+      <c r="B89" s="1">
+        <f t="shared" si="22"/>
+        <v>66.235047056138512</v>
+      </c>
+      <c r="C89" s="1">
+        <f t="shared" si="21"/>
+        <v>56.237304104268553</v>
+      </c>
+      <c r="D89" s="1">
+        <f t="shared" si="21"/>
+        <v>46.239561152398593</v>
+      </c>
+      <c r="E89" s="1">
+        <f t="shared" si="21"/>
+        <v>36.24181820052862</v>
+      </c>
+      <c r="F89" s="1">
+        <f t="shared" si="21"/>
+        <v>21.245203772723674</v>
+      </c>
+      <c r="G89" s="1">
+        <f t="shared" si="21"/>
+        <v>13.147031981709006</v>
+      </c>
+      <c r="H89" s="1">
+        <f t="shared" si="21"/>
+        <v>7.0484087810683285</v>
+      </c>
+      <c r="I89" s="1">
+        <f t="shared" si="21"/>
+        <v>0.94978558042765227</v>
+      </c>
+      <c r="J89" s="1">
+        <f t="shared" si="21"/>
+        <v>5.1488376202130244</v>
+      </c>
+      <c r="K89" s="1">
+        <f t="shared" si="21"/>
+        <v>11.247460820853719</v>
+      </c>
+      <c r="L89" s="1">
+        <f t="shared" si="21"/>
+        <v>20.445384336574069</v>
+      </c>
+      <c r="M89" s="1">
+        <f t="shared" si="21"/>
+        <v>26.444030107696058</v>
+      </c>
+      <c r="N89" s="1">
+        <f t="shared" si="21"/>
+        <v>29.643307852294456</v>
+      </c>
+      <c r="O89" s="1">
+        <f t="shared" si="21"/>
+        <v>32.642630737855441</v>
+      </c>
+      <c r="P89" s="1">
+        <f t="shared" si="21"/>
+        <v>38.741253938496115</v>
+      </c>
+      <c r="Q89" s="1">
+        <f t="shared" si="21"/>
+        <v>93.72884017378091</v>
+      </c>
+      <c r="R89" s="1"/>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>3200</v>
+      </c>
+      <c r="B90" s="1">
+        <f t="shared" si="22"/>
+        <v>61.986006301593783</v>
+      </c>
+      <c r="C90" s="1">
+        <f t="shared" si="22"/>
+        <v>51.988263349723816</v>
+      </c>
+      <c r="D90" s="1">
+        <f t="shared" si="22"/>
+        <v>41.990520397853857</v>
+      </c>
+      <c r="E90" s="1">
+        <f t="shared" si="22"/>
+        <v>31.992777445983887</v>
+      </c>
+      <c r="F90" s="1">
+        <f t="shared" si="22"/>
+        <v>16.996163018178937</v>
+      </c>
+      <c r="G90" s="1">
+        <f t="shared" si="22"/>
+        <v>8.8979912271642707</v>
+      </c>
+      <c r="H90" s="1">
+        <f t="shared" si="22"/>
+        <v>2.7993680265235943</v>
+      </c>
+      <c r="I90" s="1">
+        <f t="shared" si="22"/>
+        <v>3.2992551741170821</v>
+      </c>
+      <c r="J90" s="1">
+        <f t="shared" si="22"/>
+        <v>9.3978783747577594</v>
+      </c>
+      <c r="K90" s="1">
+        <f t="shared" si="22"/>
+        <v>15.496501575398455</v>
+      </c>
+      <c r="L90" s="1">
+        <f t="shared" si="22"/>
+        <v>24.694425091118802</v>
+      </c>
+      <c r="M90" s="1">
+        <f t="shared" si="22"/>
+        <v>30.693070862240795</v>
+      </c>
+      <c r="N90" s="1">
+        <f t="shared" si="22"/>
+        <v>33.892348606839192</v>
+      </c>
+      <c r="O90" s="1">
+        <f t="shared" si="22"/>
+        <v>36.891671492400178</v>
+      </c>
+      <c r="P90" s="1">
+        <f t="shared" si="22"/>
+        <v>42.990294693040852</v>
+      </c>
+      <c r="Q90" s="1">
+        <f t="shared" si="22"/>
+        <v>97.977880928325646</v>
+      </c>
+      <c r="R90" s="1"/>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>3500</v>
+      </c>
+      <c r="B91" s="1">
+        <f t="shared" si="22"/>
+        <v>55.612445169776677</v>
+      </c>
+      <c r="C91" s="1">
+        <f t="shared" si="22"/>
+        <v>45.614702217906718</v>
+      </c>
+      <c r="D91" s="1">
+        <f t="shared" si="22"/>
+        <v>35.616959266036758</v>
+      </c>
+      <c r="E91" s="1">
+        <f t="shared" si="22"/>
+        <v>25.619216314166785</v>
+      </c>
+      <c r="F91" s="1">
+        <f t="shared" si="22"/>
+        <v>10.622601886361837</v>
+      </c>
+      <c r="G91" s="1">
+        <f t="shared" si="22"/>
+        <v>2.524430095347169</v>
+      </c>
+      <c r="H91" s="1">
+        <f t="shared" si="22"/>
+        <v>3.5741931052935074</v>
+      </c>
+      <c r="I91" s="1">
+        <f t="shared" si="22"/>
+        <v>9.6728163059341838</v>
+      </c>
+      <c r="J91" s="1">
+        <f t="shared" si="22"/>
+        <v>15.771439506574861</v>
+      </c>
+      <c r="K91" s="1">
+        <f t="shared" si="22"/>
+        <v>21.870062707215556</v>
+      </c>
+      <c r="L91" s="1">
+        <f t="shared" si="22"/>
+        <v>31.067986222935904</v>
+      </c>
+      <c r="M91" s="1">
+        <f t="shared" si="22"/>
+        <v>37.066631994057893</v>
+      </c>
+      <c r="N91" s="1">
+        <f t="shared" si="22"/>
+        <v>40.265909738656291</v>
+      </c>
+      <c r="O91" s="1">
+        <f t="shared" si="22"/>
+        <v>43.265232624217276</v>
+      </c>
+      <c r="P91" s="1">
+        <f t="shared" si="22"/>
+        <v>49.363855824857957</v>
+      </c>
+      <c r="Q91" s="1">
+        <f t="shared" si="22"/>
+        <v>104.35144206014274</v>
+      </c>
+      <c r="R91" s="1"/>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>4000</v>
+      </c>
+      <c r="B92" s="1">
+        <f t="shared" si="22"/>
+        <v>44.989843283414842</v>
+      </c>
+      <c r="C92" s="1">
+        <f t="shared" si="22"/>
+        <v>34.992100331544869</v>
+      </c>
+      <c r="D92" s="1">
+        <f t="shared" si="22"/>
+        <v>24.99435737967492</v>
+      </c>
+      <c r="E92" s="1">
+        <f t="shared" si="22"/>
+        <v>14.996614427804948</v>
+      </c>
+      <c r="F92" s="1">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="G92" s="1">
+        <f t="shared" si="22"/>
+        <v>8.0981717910146678</v>
+      </c>
+      <c r="H92" s="1">
+        <f t="shared" si="22"/>
+        <v>14.196794991655343</v>
+      </c>
+      <c r="I92" s="1">
+        <f t="shared" si="22"/>
+        <v>20.295418192296019</v>
+      </c>
+      <c r="J92" s="1">
+        <f t="shared" si="22"/>
+        <v>26.394041392936696</v>
+      </c>
+      <c r="K92" s="1">
+        <f t="shared" si="22"/>
+        <v>32.492664593577395</v>
+      </c>
+      <c r="L92" s="1">
+        <f t="shared" si="22"/>
+        <v>41.690588109297742</v>
+      </c>
+      <c r="M92" s="1">
+        <f t="shared" si="22"/>
+        <v>47.689233880419749</v>
+      </c>
+      <c r="N92" s="1">
+        <f t="shared" si="22"/>
+        <v>50.888511625018126</v>
+      </c>
+      <c r="O92" s="1">
+        <f t="shared" si="22"/>
+        <v>53.887834510579133</v>
+      </c>
+      <c r="P92" s="1">
+        <f t="shared" si="22"/>
+        <v>59.986457711219792</v>
+      </c>
+      <c r="Q92" s="1">
+        <f t="shared" si="22"/>
+        <v>114.97404394650458</v>
+      </c>
+      <c r="R92" s="1"/>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1"/>
+      <c r="K93" s="1"/>
+      <c r="L93" s="1"/>
+      <c r="M93" s="1"/>
+      <c r="N93" s="1"/>
+      <c r="O93" s="1"/>
+      <c r="P93" s="1"/>
+      <c r="Q93" s="1"/>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>1</v>
+      </c>
+      <c r="B95" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>3</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>10</v>
+      </c>
+      <c r="D96">
+        <v>20</v>
+      </c>
+      <c r="E96">
+        <v>30</v>
+      </c>
+      <c r="F96">
+        <v>45</v>
+      </c>
+      <c r="G96">
+        <v>53.1</v>
+      </c>
+      <c r="H96">
+        <v>59.2</v>
+      </c>
+      <c r="I96">
+        <v>65.3</v>
+      </c>
+      <c r="J96">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="K96">
+        <v>77.5</v>
+      </c>
+      <c r="L96">
+        <v>86.7</v>
+      </c>
+      <c r="M96">
+        <v>92.7</v>
+      </c>
+      <c r="N96">
+        <v>95.9</v>
+      </c>
+      <c r="O96">
+        <v>98.9</v>
+      </c>
+      <c r="P96">
+        <v>105</v>
+      </c>
+      <c r="Q96">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>620</v>
+      </c>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+      <c r="K97" s="1"/>
+      <c r="L97" s="1"/>
+      <c r="M97" s="1"/>
+      <c r="N97" s="1"/>
+      <c r="O97" s="1"/>
+      <c r="P97" s="1"/>
+      <c r="Q97" s="1"/>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>650</v>
+      </c>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+      <c r="K98" s="1"/>
+      <c r="L98" s="1"/>
+      <c r="M98" s="1"/>
+      <c r="N98" s="1"/>
+      <c r="O98" s="1"/>
+      <c r="P98" s="1"/>
+      <c r="Q98" s="1"/>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>800</v>
+      </c>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1"/>
+      <c r="K99" s="1"/>
+      <c r="L99" s="1"/>
+      <c r="M99" s="1"/>
+      <c r="N99" s="1"/>
+      <c r="O99" s="1"/>
+      <c r="P99" s="1"/>
+      <c r="Q99" s="1"/>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>1000</v>
+      </c>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="1"/>
+      <c r="J100" s="1"/>
+      <c r="K100" s="1"/>
+      <c r="L100" s="1"/>
+      <c r="M100" s="1"/>
+      <c r="N100" s="1"/>
+      <c r="O100" s="1"/>
+      <c r="P100" s="1"/>
+      <c r="Q100" s="1"/>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>1200</v>
+      </c>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
+      <c r="J101" s="1"/>
+      <c r="K101" s="1"/>
+      <c r="L101" s="1"/>
+      <c r="M101" s="1"/>
+      <c r="N101" s="1"/>
+      <c r="O101" s="1"/>
+      <c r="P101" s="1"/>
+      <c r="Q101" s="1"/>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>1400</v>
+      </c>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1"/>
+      <c r="K102" s="1"/>
+      <c r="L102" s="1"/>
+      <c r="M102" s="1"/>
+      <c r="N102" s="1"/>
+      <c r="O102" s="1"/>
+      <c r="P102" s="1"/>
+      <c r="Q102" s="1"/>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>1550</v>
+      </c>
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="1"/>
+      <c r="H103" s="1"/>
+      <c r="I103" s="1"/>
+      <c r="J103" s="1"/>
+      <c r="K103" s="1"/>
+      <c r="L103" s="1"/>
+      <c r="M103" s="1"/>
+      <c r="N103" s="1"/>
+      <c r="O103" s="1"/>
+      <c r="P103" s="1"/>
+      <c r="Q103" s="1"/>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>1700</v>
+      </c>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="I104" s="1"/>
+      <c r="J104" s="1"/>
+      <c r="K104" s="1"/>
+      <c r="L104" s="1"/>
+      <c r="M104" s="1"/>
+      <c r="N104" s="1"/>
+      <c r="O104" s="1"/>
+      <c r="P104" s="1"/>
+      <c r="Q104" s="1"/>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>1800</v>
+      </c>
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="I105" s="1"/>
+      <c r="J105" s="1"/>
+      <c r="K105" s="1"/>
+      <c r="L105" s="1"/>
+      <c r="M105" s="1"/>
+      <c r="N105" s="1"/>
+      <c r="O105" s="1"/>
+      <c r="P105" s="1"/>
+      <c r="Q105" s="1"/>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>2000</v>
+      </c>
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1"/>
+      <c r="F106" s="1"/>
+      <c r="G106" s="1"/>
+      <c r="H106" s="1"/>
+      <c r="I106" s="1"/>
+      <c r="J106" s="1"/>
+      <c r="K106" s="1"/>
+      <c r="L106" s="1"/>
+      <c r="M106" s="1"/>
+      <c r="N106" s="1"/>
+      <c r="O106" s="1"/>
+      <c r="P106" s="1"/>
+      <c r="Q106" s="1"/>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>2200</v>
+      </c>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1"/>
+      <c r="F107" s="1"/>
+      <c r="G107" s="1"/>
+      <c r="H107" s="1"/>
+      <c r="I107" s="1"/>
+      <c r="J107" s="1"/>
+      <c r="K107" s="1"/>
+      <c r="L107" s="1"/>
+      <c r="M107" s="1"/>
+      <c r="N107" s="1"/>
+      <c r="O107" s="1"/>
+      <c r="P107" s="1"/>
+      <c r="Q107" s="1"/>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>2400</v>
+      </c>
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1"/>
+      <c r="F108" s="1"/>
+      <c r="G108" s="1"/>
+      <c r="H108" s="1"/>
+      <c r="I108" s="1"/>
+      <c r="J108" s="1"/>
+      <c r="K108" s="1"/>
+      <c r="L108" s="1"/>
+      <c r="M108" s="1"/>
+      <c r="N108" s="1"/>
+      <c r="O108" s="1"/>
+      <c r="P108" s="1"/>
+      <c r="Q108" s="1"/>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>2600</v>
+      </c>
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
+      <c r="D109" s="1"/>
+      <c r="E109" s="1"/>
+      <c r="F109" s="1"/>
+      <c r="G109" s="1"/>
+      <c r="H109" s="1"/>
+      <c r="I109" s="1"/>
+      <c r="J109" s="1"/>
+      <c r="K109" s="1"/>
+      <c r="L109" s="1"/>
+      <c r="M109" s="1"/>
+      <c r="N109" s="1"/>
+      <c r="O109" s="1"/>
+      <c r="P109" s="1"/>
+      <c r="Q109" s="1"/>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>2800</v>
+      </c>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1"/>
+      <c r="E110" s="1"/>
+      <c r="F110" s="1"/>
+      <c r="G110" s="1"/>
+      <c r="H110" s="1"/>
+      <c r="I110" s="1"/>
+      <c r="J110" s="1"/>
+      <c r="K110" s="1"/>
+      <c r="L110" s="1"/>
+      <c r="M110" s="1"/>
+      <c r="N110" s="1"/>
+      <c r="O110" s="1"/>
+      <c r="P110" s="1"/>
+      <c r="Q110" s="1"/>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>2900</v>
+      </c>
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
+      <c r="D111" s="1"/>
+      <c r="E111" s="1"/>
+      <c r="F111" s="1"/>
+      <c r="G111" s="1"/>
+      <c r="H111" s="1"/>
+      <c r="I111" s="1"/>
+      <c r="J111" s="1"/>
+      <c r="K111" s="1"/>
+      <c r="L111" s="1"/>
+      <c r="M111" s="1"/>
+      <c r="N111" s="1"/>
+      <c r="O111" s="1"/>
+      <c r="P111" s="1"/>
+      <c r="Q111" s="1"/>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>3000</v>
+      </c>
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
+      <c r="D112" s="1"/>
+      <c r="E112" s="1"/>
+      <c r="F112" s="1"/>
+      <c r="G112" s="1"/>
+      <c r="H112" s="1"/>
+      <c r="I112" s="1"/>
+      <c r="J112" s="1"/>
+      <c r="K112" s="1"/>
+      <c r="L112" s="1"/>
+      <c r="M112" s="1"/>
+      <c r="N112" s="1"/>
+      <c r="O112" s="1"/>
+      <c r="P112" s="1"/>
+      <c r="Q112" s="1"/>
+    </row>
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>3200</v>
+      </c>
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
+      <c r="D113" s="1"/>
+      <c r="E113" s="1"/>
+      <c r="F113" s="1"/>
+      <c r="G113" s="1"/>
+      <c r="H113" s="1"/>
+      <c r="I113" s="1"/>
+      <c r="J113" s="1"/>
+      <c r="K113" s="1"/>
+      <c r="L113" s="1"/>
+      <c r="M113" s="1"/>
+      <c r="N113" s="1"/>
+      <c r="O113" s="1"/>
+      <c r="P113" s="1"/>
+      <c r="Q113" s="1"/>
+    </row>
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>3500</v>
+      </c>
+      <c r="B114" s="1"/>
+      <c r="C114" s="1"/>
+      <c r="D114" s="1"/>
+      <c r="E114" s="1"/>
+      <c r="F114" s="1"/>
+      <c r="G114" s="1"/>
+      <c r="H114" s="1"/>
+      <c r="I114" s="1"/>
+      <c r="J114" s="1"/>
+      <c r="K114" s="1"/>
+      <c r="L114" s="1"/>
+      <c r="M114" s="1"/>
+      <c r="N114" s="1"/>
+      <c r="O114" s="1"/>
+      <c r="P114" s="1"/>
+      <c r="Q114" s="1"/>
+    </row>
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>4000</v>
+      </c>
+      <c r="B115" s="1"/>
+      <c r="C115" s="1"/>
+      <c r="D115" s="1"/>
+      <c r="E115" s="1"/>
+      <c r="F115" s="1"/>
+      <c r="G115" s="1"/>
+      <c r="H115" s="1"/>
+      <c r="I115" s="1"/>
+      <c r="J115" s="1"/>
+      <c r="K115" s="1"/>
+      <c r="L115" s="1"/>
+      <c r="M115" s="1"/>
+      <c r="N115" s="1"/>
+      <c r="O115" s="1"/>
+      <c r="P115" s="1"/>
+      <c r="Q115" s="1"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B50:Q68">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69:Q69">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="between">
+      <formula>$U$50</formula>
+      <formula>$U$51</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R50:R68">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="between">
+      <formula>$T$50</formula>
+      <formula>$T$51</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B74:Q92">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -4244,16 +6203,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B69:Q69">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
-      <formula>$U$50</formula>
-      <formula>$U$51</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R50:R68">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
-      <formula>$T$50</formula>
-      <formula>$T$51</formula>
+  <conditionalFormatting sqref="B97:Q115">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>